<commit_message>
all the files correctly saved
</commit_message>
<xml_diff>
--- a/A01_pixell_test_plan_client.xlsx
+++ b/A01_pixell_test_plan_client.xlsx
@@ -147,19 +147,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -402,61 +396,61 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -465,10 +459,10 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -834,7 +828,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="1"/>
       <c r="B3" s="8" t="s">
         <v>2</v>
@@ -1109,7 +1103,7 @@
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="31.149999999999995">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1"/>
       <c r="B18" s="21">
         <v>12</v>
@@ -1120,7 +1114,7 @@
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="31.149999999999995" customFormat="1" s="23">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="23">
       <c r="A19" s="24"/>
       <c r="B19" s="18">
         <v>13</v>

</xml_diff>